<commit_message>
Added checks from 'All' tab
</commit_message>
<xml_diff>
--- a/DataFiles/DataTables.xlsx
+++ b/DataFiles/DataTables.xlsx
@@ -35,10 +35,10 @@
     <t>ESH7</t>
   </si>
   <si>
-    <t>OEW4 Feb 24, 2017</t>
+    <t>DtExpiration</t>
   </si>
   <si>
-    <t>DtExpiration</t>
+    <t>OEW Feb 28, 2017</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +393,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -401,10 +401,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2">
-        <v>42790</v>
+        <v>42794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>